<commit_message>
Atualização Ponto de Função
Realização do cálculo
</commit_message>
<xml_diff>
--- a/Documentos de especificação complementar/Ponto de Função.xlsx
+++ b/Documentos de especificação complementar/Ponto de Função.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="12915" windowHeight="4905"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="12915" windowHeight="4905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="5" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Questões" sheetId="4" r:id="rId4"/>
     <sheet name="Coeficientes" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -276,7 +276,7 @@
     <t>Tempo para desenvolvimento</t>
   </si>
   <si>
-    <t>Os Arquivos Lógicos Internos são atualizados online?</t>
+    <t>Os Arquivos Lógicos Internos são atualizados online</t>
   </si>
 </sst>
 </file>
@@ -1337,33 +1337,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1379,16 +1352,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1431,7 +1431,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1754,7 +1794,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1764,7 +1804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -1795,7 +1835,7 @@
       <c r="E2" s="77"/>
       <c r="F2" s="59">
         <f>'Cálculo do Ponto de Função'!C8</f>
-        <v>16.900000000000002</v>
+        <v>23.92</v>
       </c>
       <c r="G2" s="60" t="s">
         <v>34</v>
@@ -1827,7 +1867,7 @@
       <c r="E4" s="80"/>
       <c r="F4" s="61">
         <f>'Cálculo do Ponto de Função'!B17</f>
-        <v>1.6900000000000002</v>
+        <v>2.3920000000000003</v>
       </c>
       <c r="G4" s="58" t="s">
         <v>39</v>
@@ -1843,7 +1883,7 @@
       <c r="E5" s="83"/>
       <c r="F5" s="70">
         <f>'Cálculo do Ponto de Função'!B19</f>
-        <v>28917.505500000003</v>
+        <v>40929.392400000004</v>
       </c>
       <c r="G5" s="71"/>
     </row>
@@ -1932,7 +1972,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,7 +2034,7 @@
       <c r="B7" s="97"/>
       <c r="C7" s="35">
         <f>Questões!E19</f>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -2004,7 +2044,7 @@
       <c r="B8" s="101"/>
       <c r="C8" s="54">
         <f>C6*(Coeficientes!A8 + (Coeficientes!A9 * C7))</f>
-        <v>16.900000000000002</v>
+        <v>23.92</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2052,7 +2092,7 @@
       </c>
       <c r="B17" s="46">
         <f>C8/B13</f>
-        <v>1.6900000000000002</v>
+        <v>2.3920000000000003</v>
       </c>
       <c r="C17" s="57" t="s">
         <v>39</v>
@@ -2065,7 +2105,7 @@
       </c>
       <c r="B19" s="56">
         <f>B12*B17*B15</f>
-        <v>28917.505500000003</v>
+        <v>40929.392400000004</v>
       </c>
     </row>
   </sheetData>
@@ -2257,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,11 +2308,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="114"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="121"/>
       <c r="E1" s="33" t="s">
         <v>27</v>
       </c>
@@ -2284,10 +2324,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="115"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="117"/>
+    <row r="2" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="122"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="8">
         <v>0</v>
       </c>
@@ -2308,25 +2348,29 @@
       </c>
     </row>
     <row r="3" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="126" t="s">
+      <c r="B3" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
       <c r="G3" s="31"/>
       <c r="H3" s="31"/>
       <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
+      <c r="J3" s="31">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="29"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="29">
+        <v>1</v>
+      </c>
       <c r="F4" s="29"/>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
@@ -2334,12 +2378,14 @@
       <c r="J4" s="29"/>
     </row>
     <row r="5" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="125"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="29">
+        <v>1</v>
+      </c>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -2347,38 +2393,44 @@
       <c r="J5" s="29"/>
     </row>
     <row r="6" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="H6" s="29">
+        <v>1</v>
+      </c>
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
     </row>
     <row r="7" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="G7" s="29">
+        <v>1</v>
+      </c>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
     </row>
     <row r="8" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="124" t="s">
+      <c r="B8" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="29"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="29">
+        <v>1</v>
+      </c>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
       <c r="H8" s="29"/>
@@ -2386,12 +2438,14 @@
       <c r="J8" s="29"/>
     </row>
     <row r="9" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="124" t="s">
+      <c r="B9" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="29"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="29">
+        <v>1</v>
+      </c>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="H9" s="29"/>
@@ -2399,12 +2453,14 @@
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="124" t="s">
+      <c r="B10" s="115" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="29"/>
+      <c r="C10" s="116"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="29">
+        <v>1</v>
+      </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
@@ -2412,104 +2468,116 @@
       <c r="J10" s="29"/>
     </row>
     <row r="11" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="124" t="s">
+      <c r="B11" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
       <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="F11" s="29">
+        <v>1</v>
+      </c>
       <c r="G11" s="29"/>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
       <c r="J11" s="29"/>
     </row>
     <row r="12" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="124" t="s">
+      <c r="B12" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
       <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="F12" s="29">
+        <v>1</v>
+      </c>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
       <c r="J12" s="29"/>
     </row>
     <row r="13" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="124" t="s">
+      <c r="B13" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
+      <c r="G13" s="29">
+        <v>1</v>
+      </c>
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
     </row>
     <row r="14" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
+      <c r="J14" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="2:10" s="24" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="124" t="s">
+      <c r="B15" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="125"/>
-      <c r="D15" s="125"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
+      <c r="J15" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="2:10" s="24" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="128" t="s">
+      <c r="B16" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="129"/>
-      <c r="D16" s="129"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
+      <c r="H16" s="32">
+        <v>1</v>
+      </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
     </row>
     <row r="17" spans="2:10" ht="13.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="118" t="s">
+      <c r="B17" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="119"/>
-      <c r="D17" s="120"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="127"/>
       <c r="E17" s="28">
         <f>SUM(E3:E16)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F17" s="26">
         <f t="shared" ref="F17:I17" si="0">SUM(F3:F16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H17" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" s="26">
         <f t="shared" si="0"/>
@@ -2517,30 +2585,30 @@
       </c>
       <c r="J17" s="27">
         <f>SUM(J3:J16)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="118" t="s">
+      <c r="B18" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="119"/>
-      <c r="D18" s="120"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="127"/>
       <c r="E18" s="28">
         <f>E17*E2</f>
         <v>0</v>
       </c>
       <c r="F18" s="26">
         <f t="shared" ref="F18:J18" si="1">F17*F2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I18" s="26">
         <f t="shared" si="1"/>
@@ -2548,27 +2616,30 @@
       </c>
       <c r="J18" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="122"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="121">
+      <c r="C19" s="113"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="112">
         <f>SUM(E18:J18)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="122"/>
-      <c r="G19" s="122"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="123"/>
+        <v>27</v>
+      </c>
+      <c r="F19" s="113"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="E19:J19"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
@@ -2585,15 +2656,12 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:J16">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>